<commit_message>
完善linux-ls命令 Signed-off-by: componey_qss <475185283@qq.com>
</commit_message>
<xml_diff>
--- a/linux/ls-rm-文件系统.xlsx
+++ b/linux/ls-rm-文件系统.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E123FAE2-4160-4618-9A2E-593A10463897}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -18,15 +19,180 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>作者</author>
+  </authors>
+  <commentList>
+    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{F3F4996B-26DB-476B-88F0-6DA8AD0818F9}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">作者:
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+  <si>
+    <t>命令格式</t>
+  </si>
+  <si>
+    <t>ls [选项] [目录名]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>命令功能</t>
+  </si>
+  <si>
+    <t>列出目标目录中所有的子目录和文件。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>常用选项/参数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>-A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>-a/-all</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>列出目录下的所有文件，包括以 . 开头的隐含文件</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>但不列出“.”(表示当前目录)和“..”(表示当前目录的父目录)。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>-h</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>以容易理解的格式列出文件大小 (例如 1K 234M 2G)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>-i</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>印出每个文件的 inode 号(即好像是每个文件夹的编号)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>-l</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>除了文件名之外，还将文件的权限、所有者、文件大小等信息详细列出来。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>和-l相同。但没有[所有者]信息。即没有群组信息</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>-g/-o</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>-R</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>同时列出所有子目录层</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>-1（数字1）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>每行只列出一个文件</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>--v/version</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>--help</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>显示此帮助信息并离开</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>显示版本信息并离开</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>优秀链接</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://blog.csdn.net/xieganyu3460/article/details/82284612</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF4F4F4F"/>
+      <name val="微软雅黑"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="微软雅黑"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="2">
@@ -49,11 +215,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -330,13 +509,283 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:P20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P18" sqref="P18"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="20.25" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="16.875" style="5" customWidth="1"/>
+    <col min="2" max="2" width="9" style="2"/>
+    <col min="3" max="16" width="9" style="4"/>
+    <col min="17" max="16384" width="9" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A4" s="1"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A5" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A6" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A7" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A8" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A9" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A10" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A11" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A12" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A13" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A14" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A15" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="C11:N11"/>
+    <mergeCell ref="C12:N12"/>
+    <mergeCell ref="C13:N13"/>
+    <mergeCell ref="C14:N14"/>
+    <mergeCell ref="C15:N15"/>
+    <mergeCell ref="C1:N1"/>
+    <mergeCell ref="C3:N3"/>
+    <mergeCell ref="C8:N8"/>
+    <mergeCell ref="C9:N9"/>
+    <mergeCell ref="C10:N10"/>
+    <mergeCell ref="C6:N6"/>
+    <mergeCell ref="C7:N7"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>